<commit_message>
fix: New Model Training
</commit_message>
<xml_diff>
--- a/ModelTraining/Models/Bayesian/GaussianProcessRegressorBenchmark.xlsx
+++ b/ModelTraining/Models/Bayesian/GaussianProcessRegressorBenchmark.xlsx
@@ -471,13 +471,13 @@
         <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>18471.42403432114</v>
+        <v>1127265073.931482</v>
       </c>
       <c r="E2" t="n">
-        <v>8.233028791461056</v>
+        <v>1117.950775121333</v>
       </c>
       <c r="F2" t="n">
-        <v>-1065.719671774751</v>
+        <v>-93432772.57103774</v>
       </c>
     </row>
     <row r="3">
@@ -491,13 +491,13 @@
         <v>10</v>
       </c>
       <c r="D3" t="n">
-        <v>18471.42403432114</v>
+        <v>1127265073.931482</v>
       </c>
       <c r="E3" t="n">
-        <v>8.233028791461056</v>
+        <v>1117.950775121333</v>
       </c>
       <c r="F3" t="n">
-        <v>-1065.719671774751</v>
+        <v>-93432772.57103774</v>
       </c>
     </row>
     <row r="4">
@@ -511,13 +511,13 @@
         <v>100</v>
       </c>
       <c r="D4" t="n">
-        <v>18471.42403432114</v>
+        <v>1127265073.931482</v>
       </c>
       <c r="E4" t="n">
-        <v>8.233028791461056</v>
+        <v>1117.950775121333</v>
       </c>
       <c r="F4" t="n">
-        <v>-1065.719671774751</v>
+        <v>-93432772.57103774</v>
       </c>
     </row>
     <row r="5">
@@ -531,13 +531,13 @@
         <v>1</v>
       </c>
       <c r="D5" t="n">
-        <v>18471.42403432114</v>
+        <v>1127265073.931482</v>
       </c>
       <c r="E5" t="n">
-        <v>8.233028791461056</v>
+        <v>1117.950775121333</v>
       </c>
       <c r="F5" t="n">
-        <v>-1065.719671774751</v>
+        <v>-93432772.57103774</v>
       </c>
     </row>
     <row r="6">
@@ -551,13 +551,13 @@
         <v>10</v>
       </c>
       <c r="D6" t="n">
-        <v>18471.42403432114</v>
+        <v>1127265073.931482</v>
       </c>
       <c r="E6" t="n">
-        <v>8.233028791461056</v>
+        <v>1117.950775121333</v>
       </c>
       <c r="F6" t="n">
-        <v>-1065.719671774751</v>
+        <v>-93432772.57103774</v>
       </c>
     </row>
     <row r="7">
@@ -571,13 +571,13 @@
         <v>100</v>
       </c>
       <c r="D7" t="n">
-        <v>18471.42403432114</v>
+        <v>1127265073.931482</v>
       </c>
       <c r="E7" t="n">
-        <v>8.233028791461056</v>
+        <v>1117.950775121333</v>
       </c>
       <c r="F7" t="n">
-        <v>-1065.719671774751</v>
+        <v>-93432772.57103774</v>
       </c>
     </row>
     <row r="8">
@@ -591,13 +591,13 @@
         <v>1</v>
       </c>
       <c r="D8" t="n">
-        <v>18471.42403432114</v>
+        <v>1127265073.931482</v>
       </c>
       <c r="E8" t="n">
-        <v>8.233028791461056</v>
+        <v>1117.950775121333</v>
       </c>
       <c r="F8" t="n">
-        <v>-1065.719671774751</v>
+        <v>-93432772.57103774</v>
       </c>
     </row>
     <row r="9">
@@ -611,13 +611,13 @@
         <v>10</v>
       </c>
       <c r="D9" t="n">
-        <v>18471.42403432114</v>
+        <v>1127265073.931482</v>
       </c>
       <c r="E9" t="n">
-        <v>8.233028791461056</v>
+        <v>1117.950775121333</v>
       </c>
       <c r="F9" t="n">
-        <v>-1065.719671774751</v>
+        <v>-93432772.57103774</v>
       </c>
     </row>
     <row r="10">
@@ -631,13 +631,13 @@
         <v>100</v>
       </c>
       <c r="D10" t="n">
-        <v>18471.42403432114</v>
+        <v>1127265073.931482</v>
       </c>
       <c r="E10" t="n">
-        <v>8.233028791461056</v>
+        <v>1117.950775121333</v>
       </c>
       <c r="F10" t="n">
-        <v>-1065.719671774751</v>
+        <v>-93432772.57103774</v>
       </c>
     </row>
   </sheetData>

</xml_diff>